<commit_message>
Correcion de listado de repuestos
</commit_message>
<xml_diff>
--- a/Repuestos.xlsx
+++ b/Repuestos.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6BB6038-2276-4D37-864A-4A8F1A04DC30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A6E5E1-0098-43CB-83EC-9C186BF50040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="340" yWindow="1280" windowWidth="16990" windowHeight="9140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -6941,10 +6941,7 @@
   <autoFilter ref="A1:F2930" xr:uid="{F6E4FAA2-237A-4AB6-A0BD-81303360F4A1}">
     <filterColumn colId="0">
       <filters>
-        <filter val="H4-HO01"/>
-        <filter val="P1-PR01"/>
-        <filter val="P1-PR01-CA01"/>
-        <filter val="P1-PR04"/>
+        <filter val="P1-PR01-ME01"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -7284,8 +7281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2930"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1855" workbookViewId="0">
-      <selection activeCell="B1546" sqref="B1546"/>
+    <sheetView tabSelected="1" topLeftCell="A1601" workbookViewId="0">
+      <selection activeCell="B2494" sqref="B2494"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -27578,7 +27575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1015" spans="1:6" ht="9" customHeight="1">
+    <row r="1015" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1015" s="2" t="s">
         <v>773</v>
       </c>
@@ -27598,7 +27595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1016" spans="1:6" ht="10" customHeight="1">
+    <row r="1016" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1016" s="2" t="s">
         <v>773</v>
       </c>
@@ -27618,7 +27615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1017" spans="1:6" ht="10" customHeight="1">
+    <row r="1017" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1017" s="2" t="s">
         <v>773</v>
       </c>
@@ -27638,7 +27635,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="1018" spans="1:6" ht="10" customHeight="1">
+    <row r="1018" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1018" s="2" t="s">
         <v>773</v>
       </c>
@@ -27658,7 +27655,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="1019" spans="1:6" ht="10" customHeight="1">
+    <row r="1019" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1019" s="2" t="s">
         <v>773</v>
       </c>
@@ -27678,7 +27675,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="1020" spans="1:6" ht="10" customHeight="1">
+    <row r="1020" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1020" s="2" t="s">
         <v>773</v>
       </c>
@@ -27698,7 +27695,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="1021" spans="1:6" ht="10" customHeight="1">
+    <row r="1021" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1021" s="2" t="s">
         <v>773</v>
       </c>
@@ -27718,7 +27715,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="1022" spans="1:6" ht="10" customHeight="1">
+    <row r="1022" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1022" s="2" t="s">
         <v>773</v>
       </c>
@@ -27738,7 +27735,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="1023" spans="1:6" ht="10" customHeight="1">
+    <row r="1023" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1023" s="2" t="s">
         <v>773</v>
       </c>
@@ -27758,7 +27755,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="1024" spans="1:6" ht="10" customHeight="1">
+    <row r="1024" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1024" s="2" t="s">
         <v>773</v>
       </c>
@@ -27778,7 +27775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1025" spans="1:6" ht="10" customHeight="1">
+    <row r="1025" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1025" s="2" t="s">
         <v>773</v>
       </c>
@@ -27798,7 +27795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1026" spans="1:6" ht="10" customHeight="1">
+    <row r="1026" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1026" s="2" t="s">
         <v>773</v>
       </c>
@@ -27818,7 +27815,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="1027" spans="1:6" ht="9" customHeight="1">
+    <row r="1027" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1027" s="2" t="s">
         <v>773</v>
       </c>
@@ -27838,7 +27835,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="1028" spans="1:6" ht="9" customHeight="1">
+    <row r="1028" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1028" s="2" t="s">
         <v>773</v>
       </c>
@@ -27858,7 +27855,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="1029" spans="1:6" ht="10" customHeight="1">
+    <row r="1029" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1029" s="2" t="s">
         <v>773</v>
       </c>
@@ -27878,7 +27875,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="1030" spans="1:6" ht="9" customHeight="1">
+    <row r="1030" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1030" s="2" t="s">
         <v>773</v>
       </c>
@@ -27898,7 +27895,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1031" spans="1:6" ht="9" customHeight="1">
+    <row r="1031" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1031" s="2" t="s">
         <v>773</v>
       </c>
@@ -27918,7 +27915,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1032" spans="1:6" ht="9" customHeight="1">
+    <row r="1032" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1032" s="2" t="s">
         <v>773</v>
       </c>
@@ -27938,7 +27935,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1033" spans="1:6" ht="9" customHeight="1">
+    <row r="1033" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1033" s="2" t="s">
         <v>773</v>
       </c>
@@ -27958,7 +27955,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1034" spans="1:6" ht="9" customHeight="1">
+    <row r="1034" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1034" s="2" t="s">
         <v>773</v>
       </c>
@@ -27978,7 +27975,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1035" spans="1:6" ht="9" customHeight="1">
+    <row r="1035" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1035" s="2" t="s">
         <v>773</v>
       </c>
@@ -27998,7 +27995,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1036" spans="1:6" ht="9" customHeight="1">
+    <row r="1036" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1036" s="2" t="s">
         <v>773</v>
       </c>
@@ -28018,7 +28015,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1037" spans="1:6" ht="9" customHeight="1">
+    <row r="1037" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1037" s="2" t="s">
         <v>773</v>
       </c>
@@ -28038,7 +28035,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1038" spans="1:6" ht="9" customHeight="1">
+    <row r="1038" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1038" s="2" t="s">
         <v>773</v>
       </c>
@@ -28058,7 +28055,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="1039" spans="1:6" ht="9" customHeight="1">
+    <row r="1039" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1039" s="2" t="s">
         <v>773</v>
       </c>
@@ -28078,7 +28075,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="1040" spans="1:6" ht="9" customHeight="1">
+    <row r="1040" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1040" s="2" t="s">
         <v>773</v>
       </c>
@@ -28098,7 +28095,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1041" spans="1:6" ht="9" customHeight="1">
+    <row r="1041" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1041" s="2" t="s">
         <v>773</v>
       </c>
@@ -28118,7 +28115,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1042" spans="1:6" ht="10" customHeight="1">
+    <row r="1042" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1042" s="2" t="s">
         <v>773</v>
       </c>
@@ -28138,7 +28135,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1043" spans="1:6" ht="9" customHeight="1">
+    <row r="1043" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1043" s="2" t="s">
         <v>773</v>
       </c>
@@ -28158,7 +28155,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="1044" spans="1:6" ht="10" customHeight="1">
+    <row r="1044" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1044" s="2" t="s">
         <v>773</v>
       </c>
@@ -35058,7 +35055,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="1389" spans="1:6" ht="9" customHeight="1">
+    <row r="1389" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1389" s="2" t="s">
         <v>985</v>
       </c>
@@ -35078,7 +35075,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="1390" spans="1:6" ht="9" customHeight="1">
+    <row r="1390" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1390" s="2" t="s">
         <v>985</v>
       </c>
@@ -35098,7 +35095,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="1391" spans="1:6" ht="9" customHeight="1">
+    <row r="1391" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1391" s="2" t="s">
         <v>985</v>
       </c>
@@ -35118,7 +35115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1392" spans="1:6" ht="10" customHeight="1">
+    <row r="1392" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1392" s="2" t="s">
         <v>985</v>
       </c>
@@ -35138,7 +35135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1393" spans="1:6" ht="10" customHeight="1">
+    <row r="1393" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1393" s="2" t="s">
         <v>985</v>
       </c>
@@ -35158,7 +35155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1394" spans="1:6" ht="10" customHeight="1">
+    <row r="1394" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1394" s="2" t="s">
         <v>985</v>
       </c>
@@ -35178,7 +35175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1395" spans="1:6" ht="9" customHeight="1">
+    <row r="1395" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1395" s="2" t="s">
         <v>985</v>
       </c>
@@ -35198,7 +35195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1396" spans="1:6" ht="9" customHeight="1">
+    <row r="1396" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1396" s="2" t="s">
         <v>985</v>
       </c>
@@ -35218,7 +35215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1397" spans="1:6" ht="10" customHeight="1">
+    <row r="1397" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1397" s="2" t="s">
         <v>985</v>
       </c>
@@ -35238,7 +35235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1398" spans="1:6" ht="10" customHeight="1">
+    <row r="1398" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1398" s="2" t="s">
         <v>985</v>
       </c>
@@ -35258,7 +35255,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1399" spans="1:6" ht="10" customHeight="1">
+    <row r="1399" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1399" s="2" t="s">
         <v>985</v>
       </c>
@@ -35278,7 +35275,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1400" spans="1:6" ht="10" customHeight="1">
+    <row r="1400" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1400" s="2" t="s">
         <v>985</v>
       </c>
@@ -35298,7 +35295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1401" spans="1:6" ht="10" customHeight="1">
+    <row r="1401" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1401" s="2" t="s">
         <v>985</v>
       </c>
@@ -35318,7 +35315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1402" spans="1:6" ht="10" customHeight="1">
+    <row r="1402" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1402" s="2" t="s">
         <v>985</v>
       </c>
@@ -35338,7 +35335,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1403" spans="1:6" ht="10" customHeight="1">
+    <row r="1403" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1403" s="2" t="s">
         <v>985</v>
       </c>
@@ -35358,7 +35355,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1404" spans="1:6" ht="10" customHeight="1">
+    <row r="1404" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1404" s="2" t="s">
         <v>985</v>
       </c>
@@ -35378,7 +35375,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1405" spans="1:6" ht="10" customHeight="1">
+    <row r="1405" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1405" s="2" t="s">
         <v>985</v>
       </c>
@@ -35398,7 +35395,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1406" spans="1:6" ht="10" customHeight="1">
+    <row r="1406" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1406" s="2" t="s">
         <v>985</v>
       </c>
@@ -35418,7 +35415,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1407" spans="1:6" ht="10" customHeight="1">
+    <row r="1407" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1407" s="2" t="s">
         <v>985</v>
       </c>
@@ -35438,7 +35435,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1408" spans="1:6" ht="10" customHeight="1">
+    <row r="1408" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1408" s="2" t="s">
         <v>985</v>
       </c>
@@ -35458,7 +35455,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1409" spans="1:6" ht="10" customHeight="1">
+    <row r="1409" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1409" s="2" t="s">
         <v>985</v>
       </c>
@@ -35478,7 +35475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1410" spans="1:6" ht="10.5" customHeight="1">
+    <row r="1410" spans="1:6" ht="10.5" hidden="1" customHeight="1">
       <c r="A1410" s="2" t="s">
         <v>985</v>
       </c>
@@ -35498,7 +35495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1411" spans="1:6" ht="10" customHeight="1">
+    <row r="1411" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1411" s="2" t="s">
         <v>985</v>
       </c>
@@ -35518,7 +35515,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1412" spans="1:6" ht="9.5" customHeight="1">
+    <row r="1412" spans="1:6" ht="9.5" hidden="1" customHeight="1">
       <c r="A1412" s="2" t="s">
         <v>985</v>
       </c>
@@ -35538,7 +35535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1413" spans="1:6" ht="10.5" customHeight="1">
+    <row r="1413" spans="1:6" ht="10.5" hidden="1" customHeight="1">
       <c r="A1413" s="2" t="s">
         <v>985</v>
       </c>
@@ -35558,7 +35555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1414" spans="1:6" ht="10" customHeight="1">
+    <row r="1414" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1414" s="2" t="s">
         <v>985</v>
       </c>
@@ -35578,7 +35575,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1415" spans="1:6" ht="10" customHeight="1">
+    <row r="1415" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1415" s="2" t="s">
         <v>985</v>
       </c>
@@ -35598,7 +35595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1416" spans="1:6" ht="10" customHeight="1">
+    <row r="1416" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1416" s="2" t="s">
         <v>985</v>
       </c>
@@ -35618,7 +35615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1417" spans="1:6" ht="10" customHeight="1">
+    <row r="1417" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1417" s="2" t="s">
         <v>985</v>
       </c>
@@ -35638,7 +35635,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1418" spans="1:6" ht="10" customHeight="1">
+    <row r="1418" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1418" s="2" t="s">
         <v>985</v>
       </c>
@@ -35658,7 +35655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1419" spans="1:6" ht="10" customHeight="1">
+    <row r="1419" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1419" s="2" t="s">
         <v>985</v>
       </c>
@@ -35678,7 +35675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1420" spans="1:6" ht="10" customHeight="1">
+    <row r="1420" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1420" s="2" t="s">
         <v>985</v>
       </c>
@@ -35698,7 +35695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1421" spans="1:6" ht="10" customHeight="1">
+    <row r="1421" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1421" s="2" t="s">
         <v>985</v>
       </c>
@@ -35718,7 +35715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1422" spans="1:6" ht="9" customHeight="1">
+    <row r="1422" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1422" s="2" t="s">
         <v>985</v>
       </c>
@@ -35738,7 +35735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1423" spans="1:6" ht="10" customHeight="1">
+    <row r="1423" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1423" s="2" t="s">
         <v>985</v>
       </c>
@@ -35758,7 +35755,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1424" spans="1:6" ht="10" customHeight="1">
+    <row r="1424" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1424" s="2" t="s">
         <v>985</v>
       </c>
@@ -35778,7 +35775,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="1425" spans="1:6" ht="10" customHeight="1">
+    <row r="1425" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1425" s="2" t="s">
         <v>985</v>
       </c>
@@ -35798,7 +35795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1426" spans="1:6" ht="9" customHeight="1">
+    <row r="1426" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1426" s="2" t="s">
         <v>985</v>
       </c>
@@ -35818,7 +35815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1427" spans="1:6" ht="10" customHeight="1">
+    <row r="1427" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1427" s="2" t="s">
         <v>985</v>
       </c>
@@ -35838,7 +35835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1428" spans="1:6" ht="10" customHeight="1">
+    <row r="1428" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1428" s="2" t="s">
         <v>985</v>
       </c>
@@ -35858,7 +35855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1429" spans="1:6" ht="10" customHeight="1">
+    <row r="1429" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1429" s="2" t="s">
         <v>985</v>
       </c>
@@ -35878,7 +35875,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1430" spans="1:6" ht="10" customHeight="1">
+    <row r="1430" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1430" s="2" t="s">
         <v>985</v>
       </c>
@@ -35898,7 +35895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1431" spans="1:6" ht="10" customHeight="1">
+    <row r="1431" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1431" s="2" t="s">
         <v>985</v>
       </c>
@@ -35918,7 +35915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1432" spans="1:6" ht="9" customHeight="1">
+    <row r="1432" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1432" s="2" t="s">
         <v>985</v>
       </c>
@@ -35938,7 +35935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1433" spans="1:6" ht="10" customHeight="1">
+    <row r="1433" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1433" s="2" t="s">
         <v>985</v>
       </c>
@@ -35958,7 +35955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1434" spans="1:6" ht="9" customHeight="1">
+    <row r="1434" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1434" s="2" t="s">
         <v>985</v>
       </c>
@@ -35978,7 +35975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1435" spans="1:6" ht="9" customHeight="1">
+    <row r="1435" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1435" s="2" t="s">
         <v>985</v>
       </c>
@@ -35998,7 +35995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1436" spans="1:6" ht="10" customHeight="1">
+    <row r="1436" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1436" s="2" t="s">
         <v>985</v>
       </c>
@@ -36018,7 +36015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1437" spans="1:6" ht="10" customHeight="1">
+    <row r="1437" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1437" s="2" t="s">
         <v>985</v>
       </c>
@@ -36038,7 +36035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1438" spans="1:6" ht="10" customHeight="1">
+    <row r="1438" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1438" s="2" t="s">
         <v>985</v>
       </c>
@@ -36058,7 +36055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1439" spans="1:6" ht="10" customHeight="1">
+    <row r="1439" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1439" s="2" t="s">
         <v>985</v>
       </c>
@@ -36078,7 +36075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1440" spans="1:6" ht="10" customHeight="1">
+    <row r="1440" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1440" s="2" t="s">
         <v>985</v>
       </c>
@@ -36098,7 +36095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1441" spans="1:6" ht="10" customHeight="1">
+    <row r="1441" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1441" s="2" t="s">
         <v>985</v>
       </c>
@@ -36118,7 +36115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1442" spans="1:6" ht="10" customHeight="1">
+    <row r="1442" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1442" s="2" t="s">
         <v>985</v>
       </c>
@@ -36138,7 +36135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1443" spans="1:6" ht="10" customHeight="1">
+    <row r="1443" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1443" s="2" t="s">
         <v>985</v>
       </c>
@@ -36158,7 +36155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1444" spans="1:6" ht="10" customHeight="1">
+    <row r="1444" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1444" s="2" t="s">
         <v>985</v>
       </c>
@@ -36178,7 +36175,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1445" spans="1:6" ht="9" customHeight="1">
+    <row r="1445" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1445" s="2" t="s">
         <v>985</v>
       </c>
@@ -36198,7 +36195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1446" spans="1:6" ht="10" customHeight="1">
+    <row r="1446" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1446" s="2" t="s">
         <v>985</v>
       </c>
@@ -36218,7 +36215,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1447" spans="1:6" ht="10" customHeight="1">
+    <row r="1447" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1447" s="2" t="s">
         <v>985</v>
       </c>
@@ -36238,7 +36235,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1448" spans="1:6" ht="10" customHeight="1">
+    <row r="1448" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1448" s="2" t="s">
         <v>985</v>
       </c>
@@ -36258,7 +36255,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1449" spans="1:6" ht="10" customHeight="1">
+    <row r="1449" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1449" s="2" t="s">
         <v>985</v>
       </c>
@@ -36278,7 +36275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1450" spans="1:6" ht="9" customHeight="1">
+    <row r="1450" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1450" s="2" t="s">
         <v>985</v>
       </c>
@@ -36298,7 +36295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1451" spans="1:6" ht="9" customHeight="1">
+    <row r="1451" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1451" s="2" t="s">
         <v>985</v>
       </c>
@@ -36318,7 +36315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1452" spans="1:6" ht="10" customHeight="1">
+    <row r="1452" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1452" s="2" t="s">
         <v>985</v>
       </c>
@@ -36338,7 +36335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1453" spans="1:6" ht="10" customHeight="1">
+    <row r="1453" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1453" s="2" t="s">
         <v>985</v>
       </c>
@@ -36358,7 +36355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1454" spans="1:6" ht="10" customHeight="1">
+    <row r="1454" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1454" s="2" t="s">
         <v>985</v>
       </c>
@@ -36378,7 +36375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1455" spans="1:6" ht="10" customHeight="1">
+    <row r="1455" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1455" s="2" t="s">
         <v>985</v>
       </c>
@@ -36398,7 +36395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1456" spans="1:6" ht="9" customHeight="1">
+    <row r="1456" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1456" s="2" t="s">
         <v>985</v>
       </c>
@@ -36418,7 +36415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1457" spans="1:6" ht="10" customHeight="1">
+    <row r="1457" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1457" s="2" t="s">
         <v>985</v>
       </c>
@@ -36438,7 +36435,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1458" spans="1:6" ht="9" customHeight="1">
+    <row r="1458" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1458" s="2" t="s">
         <v>985</v>
       </c>
@@ -36458,7 +36455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1459" spans="1:6" ht="10" customHeight="1">
+    <row r="1459" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1459" s="2" t="s">
         <v>985</v>
       </c>
@@ -36478,7 +36475,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="1460" spans="1:6" ht="10" customHeight="1">
+    <row r="1460" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1460" s="2" t="s">
         <v>985</v>
       </c>
@@ -36498,7 +36495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1461" spans="1:6" ht="10" customHeight="1">
+    <row r="1461" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1461" s="2" t="s">
         <v>985</v>
       </c>
@@ -36518,7 +36515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1462" spans="1:6" ht="10" customHeight="1">
+    <row r="1462" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1462" s="2" t="s">
         <v>985</v>
       </c>
@@ -36538,7 +36535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1463" spans="1:6" ht="10" customHeight="1">
+    <row r="1463" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1463" s="2" t="s">
         <v>985</v>
       </c>
@@ -36558,7 +36555,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1464" spans="1:6" ht="9" customHeight="1">
+    <row r="1464" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1464" s="2" t="s">
         <v>985</v>
       </c>
@@ -36578,7 +36575,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1465" spans="1:6" ht="9" customHeight="1">
+    <row r="1465" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1465" s="2" t="s">
         <v>985</v>
       </c>
@@ -36598,7 +36595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1466" spans="1:6" ht="10" customHeight="1">
+    <row r="1466" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1466" s="2" t="s">
         <v>985</v>
       </c>
@@ -36618,7 +36615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1467" spans="1:6" ht="10" customHeight="1">
+    <row r="1467" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1467" s="2" t="s">
         <v>985</v>
       </c>
@@ -36638,7 +36635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1468" spans="1:6" ht="10" customHeight="1">
+    <row r="1468" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1468" s="2" t="s">
         <v>985</v>
       </c>
@@ -36658,7 +36655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1469" spans="1:6" ht="10" customHeight="1">
+    <row r="1469" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1469" s="2" t="s">
         <v>985</v>
       </c>
@@ -36678,7 +36675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1470" spans="1:6" ht="10" customHeight="1">
+    <row r="1470" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1470" s="2" t="s">
         <v>985</v>
       </c>
@@ -36698,7 +36695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1471" spans="1:6" ht="10" customHeight="1">
+    <row r="1471" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1471" s="2" t="s">
         <v>985</v>
       </c>
@@ -36718,7 +36715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1472" spans="1:6" ht="10" customHeight="1">
+    <row r="1472" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1472" s="2" t="s">
         <v>985</v>
       </c>
@@ -36738,7 +36735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1473" spans="1:6" ht="10" customHeight="1">
+    <row r="1473" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1473" s="2" t="s">
         <v>985</v>
       </c>
@@ -36758,7 +36755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1474" spans="1:6" ht="10" customHeight="1">
+    <row r="1474" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1474" s="2" t="s">
         <v>985</v>
       </c>
@@ -36778,7 +36775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1475" spans="1:6" ht="9" customHeight="1">
+    <row r="1475" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1475" s="2" t="s">
         <v>985</v>
       </c>
@@ -36798,7 +36795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1476" spans="1:6" ht="10" customHeight="1">
+    <row r="1476" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1476" s="2" t="s">
         <v>985</v>
       </c>
@@ -36818,7 +36815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1477" spans="1:6" ht="10" customHeight="1">
+    <row r="1477" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1477" s="2" t="s">
         <v>985</v>
       </c>
@@ -36838,7 +36835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1478" spans="1:6" ht="10" customHeight="1">
+    <row r="1478" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1478" s="2" t="s">
         <v>985</v>
       </c>
@@ -36858,7 +36855,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1479" spans="1:6" ht="10" customHeight="1">
+    <row r="1479" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1479" s="2" t="s">
         <v>985</v>
       </c>
@@ -36878,7 +36875,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1480" spans="1:6" ht="10" customHeight="1">
+    <row r="1480" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1480" s="2" t="s">
         <v>985</v>
       </c>
@@ -36898,7 +36895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1481" spans="1:6" ht="9" customHeight="1">
+    <row r="1481" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1481" s="2" t="s">
         <v>985</v>
       </c>
@@ -36918,7 +36915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1482" spans="1:6" ht="10" customHeight="1">
+    <row r="1482" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1482" s="2" t="s">
         <v>985</v>
       </c>
@@ -36938,7 +36935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1483" spans="1:6" ht="9" customHeight="1">
+    <row r="1483" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1483" s="2" t="s">
         <v>985</v>
       </c>
@@ -36958,7 +36955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1484" spans="1:6" ht="10" customHeight="1">
+    <row r="1484" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1484" s="2" t="s">
         <v>985</v>
       </c>
@@ -36978,7 +36975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1485" spans="1:6" ht="10" customHeight="1">
+    <row r="1485" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1485" s="2" t="s">
         <v>985</v>
       </c>
@@ -36998,7 +36995,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1486" spans="1:6" ht="10" customHeight="1">
+    <row r="1486" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1486" s="2" t="s">
         <v>985</v>
       </c>
@@ -37018,7 +37015,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1487" spans="1:6" ht="9" customHeight="1">
+    <row r="1487" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1487" s="2" t="s">
         <v>985</v>
       </c>
@@ -37038,7 +37035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1488" spans="1:6" ht="10" customHeight="1">
+    <row r="1488" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1488" s="2" t="s">
         <v>985</v>
       </c>
@@ -37058,7 +37055,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1489" spans="1:6" ht="10" customHeight="1">
+    <row r="1489" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1489" s="2" t="s">
         <v>985</v>
       </c>
@@ -37078,7 +37075,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1490" spans="1:6" ht="10" customHeight="1">
+    <row r="1490" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1490" s="2" t="s">
         <v>985</v>
       </c>
@@ -37098,7 +37095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1491" spans="1:6" ht="9" customHeight="1">
+    <row r="1491" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1491" s="2" t="s">
         <v>985</v>
       </c>
@@ -37118,7 +37115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1492" spans="1:6" ht="10" customHeight="1">
+    <row r="1492" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1492" s="2" t="s">
         <v>985</v>
       </c>
@@ -37138,7 +37135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1493" spans="1:6" ht="10" customHeight="1">
+    <row r="1493" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1493" s="2" t="s">
         <v>985</v>
       </c>
@@ -37158,7 +37155,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1494" spans="1:6" ht="10" customHeight="1">
+    <row r="1494" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1494" s="2" t="s">
         <v>985</v>
       </c>
@@ -37178,7 +37175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1495" spans="1:6" ht="9" customHeight="1">
+    <row r="1495" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1495" s="2" t="s">
         <v>985</v>
       </c>
@@ -37198,7 +37195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1496" spans="1:6" ht="10" customHeight="1">
+    <row r="1496" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1496" s="2" t="s">
         <v>985</v>
       </c>
@@ -37218,7 +37215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1497" spans="1:6" ht="10" customHeight="1">
+    <row r="1497" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1497" s="2" t="s">
         <v>985</v>
       </c>
@@ -37238,7 +37235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1498" spans="1:6" ht="9" customHeight="1">
+    <row r="1498" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1498" s="2" t="s">
         <v>985</v>
       </c>
@@ -37258,7 +37255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1499" spans="1:6" ht="10" customHeight="1">
+    <row r="1499" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1499" s="2" t="s">
         <v>985</v>
       </c>
@@ -37278,7 +37275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1500" spans="1:6" ht="10" customHeight="1">
+    <row r="1500" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1500" s="2" t="s">
         <v>985</v>
       </c>
@@ -37298,7 +37295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1501" spans="1:6" ht="10" customHeight="1">
+    <row r="1501" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1501" s="2" t="s">
         <v>985</v>
       </c>
@@ -37318,7 +37315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1502" spans="1:6" ht="10" customHeight="1">
+    <row r="1502" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1502" s="2" t="s">
         <v>985</v>
       </c>
@@ -37338,7 +37335,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1503" spans="1:6" ht="9" customHeight="1">
+    <row r="1503" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1503" s="2" t="s">
         <v>985</v>
       </c>
@@ -37358,7 +37355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1504" spans="1:6" ht="10" customHeight="1">
+    <row r="1504" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1504" s="2" t="s">
         <v>985</v>
       </c>
@@ -37378,7 +37375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1505" spans="1:6" ht="11" customHeight="1">
+    <row r="1505" spans="1:6" ht="11" hidden="1" customHeight="1">
       <c r="A1505" s="2" t="s">
         <v>985</v>
       </c>
@@ -37398,7 +37395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1506" spans="1:6" ht="10" customHeight="1">
+    <row r="1506" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1506" s="2" t="s">
         <v>985</v>
       </c>
@@ -37418,7 +37415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1507" spans="1:6" ht="10" customHeight="1">
+    <row r="1507" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1507" s="2" t="s">
         <v>985</v>
       </c>
@@ -37438,7 +37435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1508" spans="1:6" ht="10" customHeight="1">
+    <row r="1508" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1508" s="2" t="s">
         <v>985</v>
       </c>
@@ -37458,7 +37455,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="1509" spans="1:6" ht="10" customHeight="1">
+    <row r="1509" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1509" s="2" t="s">
         <v>985</v>
       </c>
@@ -37478,7 +37475,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1510" spans="1:6" ht="10" customHeight="1">
+    <row r="1510" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1510" s="2" t="s">
         <v>985</v>
       </c>
@@ -37498,7 +37495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1511" spans="1:6" ht="10" customHeight="1">
+    <row r="1511" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1511" s="2" t="s">
         <v>985</v>
       </c>
@@ -37518,7 +37515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1512" spans="1:6" ht="10" customHeight="1">
+    <row r="1512" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1512" s="2" t="s">
         <v>985</v>
       </c>
@@ -37538,7 +37535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1513" spans="1:6" ht="9" customHeight="1">
+    <row r="1513" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1513" s="2" t="s">
         <v>985</v>
       </c>
@@ -37558,7 +37555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1514" spans="1:6" ht="10" customHeight="1">
+    <row r="1514" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1514" s="2" t="s">
         <v>985</v>
       </c>
@@ -37578,7 +37575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1515" spans="1:6" ht="9" customHeight="1">
+    <row r="1515" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1515" s="2" t="s">
         <v>985</v>
       </c>
@@ -37598,7 +37595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1516" spans="1:6" ht="10" customHeight="1">
+    <row r="1516" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1516" s="2" t="s">
         <v>985</v>
       </c>
@@ -37618,7 +37615,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1517" spans="1:6" ht="10" customHeight="1">
+    <row r="1517" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1517" s="2" t="s">
         <v>985</v>
       </c>
@@ -37638,7 +37635,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="1518" spans="1:6" ht="10" customHeight="1">
+    <row r="1518" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1518" s="2" t="s">
         <v>985</v>
       </c>
@@ -37658,7 +37655,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="1519" spans="1:6" ht="9" customHeight="1">
+    <row r="1519" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1519" s="2" t="s">
         <v>985</v>
       </c>
@@ -37678,7 +37675,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1520" spans="1:6" ht="9" customHeight="1">
+    <row r="1520" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1520" s="2" t="s">
         <v>985</v>
       </c>
@@ -37698,7 +37695,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1521" spans="1:6" ht="9" customHeight="1">
+    <row r="1521" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1521" s="2" t="s">
         <v>985</v>
       </c>
@@ -37718,7 +37715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1522" spans="1:6" ht="9" customHeight="1">
+    <row r="1522" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1522" s="2" t="s">
         <v>985</v>
       </c>
@@ -37738,7 +37735,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="1523" spans="1:6" ht="10" customHeight="1">
+    <row r="1523" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1523" s="2" t="s">
         <v>985</v>
       </c>
@@ -37758,7 +37755,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="1524" spans="1:6" ht="9" customHeight="1">
+    <row r="1524" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1524" s="2" t="s">
         <v>985</v>
       </c>
@@ -37778,7 +37775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1525" spans="1:6" ht="10" customHeight="1">
+    <row r="1525" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1525" s="2" t="s">
         <v>985</v>
       </c>
@@ -37798,7 +37795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1526" spans="1:6" ht="10" customHeight="1">
+    <row r="1526" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1526" s="2" t="s">
         <v>985</v>
       </c>
@@ -37818,7 +37815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1527" spans="1:6" ht="10" customHeight="1">
+    <row r="1527" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1527" s="2" t="s">
         <v>985</v>
       </c>
@@ -37838,7 +37835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1528" spans="1:6" ht="10" customHeight="1">
+    <row r="1528" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1528" s="2" t="s">
         <v>985</v>
       </c>
@@ -37858,7 +37855,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1529" spans="1:6" ht="9" customHeight="1">
+    <row r="1529" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1529" s="2" t="s">
         <v>985</v>
       </c>
@@ -37878,7 +37875,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="1530" spans="1:6" ht="10" customHeight="1">
+    <row r="1530" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1530" s="2" t="s">
         <v>985</v>
       </c>
@@ -37898,7 +37895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1531" spans="1:6" ht="10" customHeight="1">
+    <row r="1531" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1531" s="2" t="s">
         <v>985</v>
       </c>
@@ -37918,7 +37915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1532" spans="1:6" ht="10" customHeight="1">
+    <row r="1532" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1532" s="2" t="s">
         <v>985</v>
       </c>
@@ -37938,7 +37935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1533" spans="1:6" ht="9" customHeight="1">
+    <row r="1533" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1533" s="2" t="s">
         <v>985</v>
       </c>
@@ -37958,7 +37955,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1534" spans="1:6" ht="9" customHeight="1">
+    <row r="1534" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1534" s="2" t="s">
         <v>985</v>
       </c>
@@ -37978,7 +37975,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1535" spans="1:6" ht="10" customHeight="1">
+    <row r="1535" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1535" s="2" t="s">
         <v>985</v>
       </c>
@@ -37998,7 +37995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1536" spans="1:6" ht="9" customHeight="1">
+    <row r="1536" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1536" s="2" t="s">
         <v>985</v>
       </c>
@@ -38018,7 +38015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1537" spans="1:6" ht="9" customHeight="1">
+    <row r="1537" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1537" s="2" t="s">
         <v>985</v>
       </c>
@@ -38038,7 +38035,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="1538" spans="1:6" ht="9" customHeight="1">
+    <row r="1538" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1538" s="2" t="s">
         <v>985</v>
       </c>
@@ -38058,7 +38055,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="1539" spans="1:6" ht="9" customHeight="1">
+    <row r="1539" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1539" s="2" t="s">
         <v>985</v>
       </c>
@@ -38078,7 +38075,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="1540" spans="1:6" ht="9" customHeight="1">
+    <row r="1540" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1540" s="2" t="s">
         <v>985</v>
       </c>
@@ -38098,7 +38095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1541" spans="1:6" ht="10" customHeight="1">
+    <row r="1541" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1541" s="2" t="s">
         <v>985</v>
       </c>
@@ -38118,7 +38115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1542" spans="1:6" ht="11" customHeight="1">
+    <row r="1542" spans="1:6" ht="11" hidden="1" customHeight="1">
       <c r="A1542" s="2" t="s">
         <v>985</v>
       </c>
@@ -38138,7 +38135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1543" spans="1:6" ht="9" customHeight="1">
+    <row r="1543" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1543" s="2" t="s">
         <v>985</v>
       </c>
@@ -38158,7 +38155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1544" spans="1:6" ht="10" customHeight="1">
+    <row r="1544" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1544" s="2" t="s">
         <v>985</v>
       </c>
@@ -38178,7 +38175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1545" spans="1:6" ht="9" customHeight="1">
+    <row r="1545" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1545" s="2" t="s">
         <v>985</v>
       </c>
@@ -38198,7 +38195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1546" spans="1:6" ht="9" customHeight="1">
+    <row r="1546" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1546" s="2" t="s">
         <v>1292</v>
       </c>
@@ -38218,7 +38215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1547" spans="1:6" ht="9" customHeight="1">
+    <row r="1547" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1547" s="2" t="s">
         <v>1292</v>
       </c>
@@ -38238,7 +38235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1548" spans="1:6" ht="9" customHeight="1">
+    <row r="1548" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1548" s="2" t="s">
         <v>1292</v>
       </c>
@@ -38258,7 +38255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1549" spans="1:6" ht="9" customHeight="1">
+    <row r="1549" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1549" s="2" t="s">
         <v>1292</v>
       </c>
@@ -38958,7 +38955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1584" spans="1:6" ht="10" hidden="1" customHeight="1">
+    <row r="1584" spans="1:6" ht="10" customHeight="1">
       <c r="A1584" s="2" t="s">
         <v>1346</v>
       </c>
@@ -38978,7 +38975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1585" spans="1:6" ht="9" hidden="1" customHeight="1">
+    <row r="1585" spans="1:6" ht="9" customHeight="1">
       <c r="A1585" s="2" t="s">
         <v>1346</v>
       </c>
@@ -38998,7 +38995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1586" spans="1:6" ht="9" hidden="1" customHeight="1">
+    <row r="1586" spans="1:6" ht="9" customHeight="1">
       <c r="A1586" s="2" t="s">
         <v>1346</v>
       </c>
@@ -39018,7 +39015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1587" spans="1:6" ht="10" hidden="1" customHeight="1">
+    <row r="1587" spans="1:6" ht="10" customHeight="1">
       <c r="A1587" s="2" t="s">
         <v>1346</v>
       </c>
@@ -39038,7 +39035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1588" spans="1:6" ht="9" hidden="1" customHeight="1">
+    <row r="1588" spans="1:6" ht="9" customHeight="1">
       <c r="A1588" s="2" t="s">
         <v>1346</v>
       </c>
@@ -39058,7 +39055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1589" spans="1:6" ht="9" hidden="1" customHeight="1">
+    <row r="1589" spans="1:6" ht="9" customHeight="1">
       <c r="A1589" s="2" t="s">
         <v>1346</v>
       </c>
@@ -39078,7 +39075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1590" spans="1:6" ht="10" hidden="1" customHeight="1">
+    <row r="1590" spans="1:6" ht="10" customHeight="1">
       <c r="A1590" s="2" t="s">
         <v>1346</v>
       </c>
@@ -39098,7 +39095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1591" spans="1:6" ht="10" hidden="1" customHeight="1">
+    <row r="1591" spans="1:6" ht="10" customHeight="1">
       <c r="A1591" s="2" t="s">
         <v>1346</v>
       </c>
@@ -39118,7 +39115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1592" spans="1:6" ht="10" hidden="1" customHeight="1">
+    <row r="1592" spans="1:6" ht="10" customHeight="1">
       <c r="A1592" s="2" t="s">
         <v>1346</v>
       </c>
@@ -39138,7 +39135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1593" spans="1:6" ht="10" hidden="1" customHeight="1">
+    <row r="1593" spans="1:6" ht="10" customHeight="1">
       <c r="A1593" s="2" t="s">
         <v>1346</v>
       </c>
@@ -39158,7 +39155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1594" spans="1:6" ht="10" hidden="1" customHeight="1">
+    <row r="1594" spans="1:6" ht="10" customHeight="1">
       <c r="A1594" s="2" t="s">
         <v>1346</v>
       </c>
@@ -39178,7 +39175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1595" spans="1:6" ht="10" hidden="1" customHeight="1">
+    <row r="1595" spans="1:6" ht="10" customHeight="1">
       <c r="A1595" s="2" t="s">
         <v>1346</v>
       </c>
@@ -39198,7 +39195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1596" spans="1:6" ht="9" hidden="1" customHeight="1">
+    <row r="1596" spans="1:6" ht="9" customHeight="1">
       <c r="A1596" s="2" t="s">
         <v>1346</v>
       </c>
@@ -39218,7 +39215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1597" spans="1:6" ht="10" hidden="1" customHeight="1">
+    <row r="1597" spans="1:6" ht="10" customHeight="1">
       <c r="A1597" s="2" t="s">
         <v>1346</v>
       </c>
@@ -39238,7 +39235,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="1598" spans="1:6" ht="9" hidden="1" customHeight="1">
+    <row r="1598" spans="1:6" ht="9" customHeight="1">
       <c r="A1598" s="2" t="s">
         <v>1346</v>
       </c>
@@ -39258,7 +39255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1599" spans="1:6" ht="9" hidden="1" customHeight="1">
+    <row r="1599" spans="1:6" ht="9" customHeight="1">
       <c r="A1599" s="2" t="s">
         <v>1346</v>
       </c>
@@ -39278,7 +39275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1600" spans="1:6" ht="9" hidden="1" customHeight="1">
+    <row r="1600" spans="1:6" ht="9" customHeight="1">
       <c r="A1600" s="2" t="s">
         <v>1346</v>
       </c>
@@ -39298,7 +39295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1601" spans="1:6" ht="10" hidden="1" customHeight="1">
+    <row r="1601" spans="1:6" ht="10" customHeight="1">
       <c r="A1601" s="2" t="s">
         <v>1346</v>
       </c>
@@ -39318,7 +39315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1602" spans="1:6" ht="9" hidden="1" customHeight="1">
+    <row r="1602" spans="1:6" ht="9" customHeight="1">
       <c r="A1602" s="2" t="s">
         <v>1346</v>
       </c>
@@ -39338,7 +39335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1603" spans="1:6" ht="10" hidden="1" customHeight="1">
+    <row r="1603" spans="1:6" ht="10" customHeight="1">
       <c r="A1603" s="2" t="s">
         <v>1346</v>
       </c>
@@ -39358,7 +39355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1604" spans="1:6" ht="10" hidden="1" customHeight="1">
+    <row r="1604" spans="1:6" ht="10" customHeight="1">
       <c r="A1604" s="2" t="s">
         <v>1346</v>
       </c>
@@ -39378,7 +39375,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1605" spans="1:6" ht="10" hidden="1" customHeight="1">
+    <row r="1605" spans="1:6" ht="10" customHeight="1">
       <c r="A1605" s="2" t="s">
         <v>1346</v>
       </c>
@@ -39398,7 +39395,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="1606" spans="1:6" ht="9" hidden="1" customHeight="1">
+    <row r="1606" spans="1:6" ht="9" customHeight="1">
       <c r="A1606" s="2" t="s">
         <v>1346</v>
       </c>
@@ -39418,7 +39415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1607" spans="1:6" ht="10" hidden="1" customHeight="1">
+    <row r="1607" spans="1:6" ht="10" customHeight="1">
       <c r="A1607" s="2" t="s">
         <v>1346</v>
       </c>
@@ -39438,7 +39435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1608" spans="1:6" ht="9" hidden="1" customHeight="1">
+    <row r="1608" spans="1:6" ht="9" customHeight="1">
       <c r="A1608" s="2" t="s">
         <v>1346</v>
       </c>
@@ -39458,7 +39455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1609" spans="1:6" ht="9" hidden="1" customHeight="1">
+    <row r="1609" spans="1:6" ht="9" customHeight="1">
       <c r="A1609" s="2" t="s">
         <v>1346</v>
       </c>
@@ -39478,7 +39475,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1610" spans="1:6" ht="9" hidden="1" customHeight="1">
+    <row r="1610" spans="1:6" ht="9" customHeight="1">
       <c r="A1610" s="2" t="s">
         <v>1346</v>
       </c>
@@ -39498,7 +39495,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1611" spans="1:6" ht="9" hidden="1" customHeight="1">
+    <row r="1611" spans="1:6" ht="9" customHeight="1">
       <c r="A1611" s="2" t="s">
         <v>1346</v>
       </c>
@@ -39518,7 +39515,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1612" spans="1:6" ht="9" hidden="1" customHeight="1">
+    <row r="1612" spans="1:6" ht="9" customHeight="1">
       <c r="A1612" s="2" t="s">
         <v>1346</v>
       </c>
@@ -39538,7 +39535,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1613" spans="1:6" ht="10" hidden="1" customHeight="1">
+    <row r="1613" spans="1:6" ht="10" customHeight="1">
       <c r="A1613" s="2" t="s">
         <v>1346</v>
       </c>
@@ -39558,7 +39555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1614" spans="1:6" ht="9" hidden="1" customHeight="1">
+    <row r="1614" spans="1:6" ht="9" customHeight="1">
       <c r="A1614" s="2" t="s">
         <v>1346</v>
       </c>
@@ -39578,7 +39575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1615" spans="1:6" ht="9" hidden="1" customHeight="1">
+    <row r="1615" spans="1:6" ht="9" customHeight="1">
       <c r="A1615" s="2" t="s">
         <v>1346</v>
       </c>
@@ -39598,7 +39595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1616" spans="1:6" ht="10" hidden="1" customHeight="1">
+    <row r="1616" spans="1:6" ht="10" customHeight="1">
       <c r="A1616" s="2" t="s">
         <v>1346</v>
       </c>
@@ -39618,7 +39615,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="1617" spans="1:6" ht="10" hidden="1" customHeight="1">
+    <row r="1617" spans="1:6" ht="10" customHeight="1">
       <c r="A1617" s="2" t="s">
         <v>1346</v>
       </c>
@@ -39638,7 +39635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1618" spans="1:6" ht="9" hidden="1" customHeight="1">
+    <row r="1618" spans="1:6" ht="9" customHeight="1">
       <c r="A1618" s="2" t="s">
         <v>1346</v>
       </c>
@@ -43918,7 +43915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1832" spans="1:6" ht="9" customHeight="1">
+    <row r="1832" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1832" s="2" t="s">
         <v>1630</v>
       </c>
@@ -43938,7 +43935,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="1833" spans="1:6" ht="9" customHeight="1">
+    <row r="1833" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1833" s="2" t="s">
         <v>1630</v>
       </c>
@@ -43958,7 +43955,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="1834" spans="1:6" ht="9" customHeight="1">
+    <row r="1834" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1834" s="2" t="s">
         <v>1630</v>
       </c>
@@ -43978,7 +43975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1835" spans="1:6" ht="10" customHeight="1">
+    <row r="1835" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1835" s="2" t="s">
         <v>1630</v>
       </c>
@@ -43998,7 +43995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1836" spans="1:6" ht="9" customHeight="1">
+    <row r="1836" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1836" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44018,7 +44015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1837" spans="1:6" ht="10" customHeight="1">
+    <row r="1837" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1837" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44038,7 +44035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1838" spans="1:6" ht="10" customHeight="1">
+    <row r="1838" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1838" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44058,7 +44055,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1839" spans="1:6" ht="10" customHeight="1">
+    <row r="1839" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1839" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44078,7 +44075,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1840" spans="1:6" ht="10" customHeight="1">
+    <row r="1840" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1840" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44098,7 +44095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1841" spans="1:6" ht="10" customHeight="1">
+    <row r="1841" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1841" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44118,7 +44115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1842" spans="1:6" ht="10" customHeight="1">
+    <row r="1842" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1842" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44138,7 +44135,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1843" spans="1:6" ht="10" customHeight="1">
+    <row r="1843" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1843" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44158,7 +44155,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1844" spans="1:6" ht="10" customHeight="1">
+    <row r="1844" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1844" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44178,7 +44175,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1845" spans="1:6" ht="10" customHeight="1">
+    <row r="1845" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1845" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44198,7 +44195,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1846" spans="1:6" ht="10" customHeight="1">
+    <row r="1846" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1846" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44218,7 +44215,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1847" spans="1:6" ht="10" customHeight="1">
+    <row r="1847" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1847" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44238,7 +44235,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1848" spans="1:6" ht="10" customHeight="1">
+    <row r="1848" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1848" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44258,7 +44255,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1849" spans="1:6" ht="10" customHeight="1">
+    <row r="1849" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1849" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44278,7 +44275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1850" spans="1:6" ht="10.5" customHeight="1">
+    <row r="1850" spans="1:6" ht="10.5" hidden="1" customHeight="1">
       <c r="A1850" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44298,7 +44295,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1851" spans="1:6" ht="10" customHeight="1">
+    <row r="1851" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1851" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44318,7 +44315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1852" spans="1:6" ht="9.5" customHeight="1">
+    <row r="1852" spans="1:6" ht="9.5" hidden="1" customHeight="1">
       <c r="A1852" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44338,7 +44335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1853" spans="1:6" ht="10.5" customHeight="1">
+    <row r="1853" spans="1:6" ht="10.5" hidden="1" customHeight="1">
       <c r="A1853" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44358,7 +44355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1854" spans="1:6" ht="10" customHeight="1">
+    <row r="1854" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1854" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44378,7 +44375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1855" spans="1:6" ht="10" customHeight="1">
+    <row r="1855" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1855" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44398,7 +44395,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1856" spans="1:6" ht="10" customHeight="1">
+    <row r="1856" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1856" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44418,7 +44415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1857" spans="1:6" ht="10" customHeight="1">
+    <row r="1857" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1857" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44438,7 +44435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1858" spans="1:6" ht="10" customHeight="1">
+    <row r="1858" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1858" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44458,7 +44455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1859" spans="1:6" ht="10" customHeight="1">
+    <row r="1859" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1859" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44478,7 +44475,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1860" spans="1:6" ht="10" customHeight="1">
+    <row r="1860" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1860" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44498,7 +44495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1861" spans="1:6" ht="10" customHeight="1">
+    <row r="1861" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1861" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44518,7 +44515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1862" spans="1:6" ht="9" customHeight="1">
+    <row r="1862" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1862" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44538,7 +44535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1863" spans="1:6" ht="10" customHeight="1">
+    <row r="1863" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1863" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44558,7 +44555,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1864" spans="1:6" ht="10" customHeight="1">
+    <row r="1864" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1864" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44578,7 +44575,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="1865" spans="1:6" ht="9" customHeight="1">
+    <row r="1865" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1865" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44598,7 +44595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1866" spans="1:6" ht="10" customHeight="1">
+    <row r="1866" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1866" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44618,7 +44615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1867" spans="1:6" ht="10" customHeight="1">
+    <row r="1867" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1867" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44638,7 +44635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1868" spans="1:6" ht="10" customHeight="1">
+    <row r="1868" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1868" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44658,7 +44655,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1869" spans="1:6" ht="10" customHeight="1">
+    <row r="1869" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1869" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44678,7 +44675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1870" spans="1:6" ht="10" customHeight="1">
+    <row r="1870" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1870" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44698,7 +44695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1871" spans="1:6" ht="9" customHeight="1">
+    <row r="1871" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1871" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44718,7 +44715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1872" spans="1:6" ht="10" customHeight="1">
+    <row r="1872" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1872" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44738,7 +44735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1873" spans="1:6" ht="9" customHeight="1">
+    <row r="1873" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1873" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44758,7 +44755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1874" spans="1:6" ht="9" customHeight="1">
+    <row r="1874" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1874" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44778,7 +44775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1875" spans="1:6" ht="10" customHeight="1">
+    <row r="1875" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1875" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44798,7 +44795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1876" spans="1:6" ht="10" customHeight="1">
+    <row r="1876" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1876" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44818,7 +44815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1877" spans="1:6" ht="10" customHeight="1">
+    <row r="1877" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1877" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44838,7 +44835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1878" spans="1:6" ht="10" customHeight="1">
+    <row r="1878" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1878" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44858,7 +44855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1879" spans="1:6" ht="10" customHeight="1">
+    <row r="1879" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1879" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44878,7 +44875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1880" spans="1:6" ht="10" customHeight="1">
+    <row r="1880" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1880" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44898,7 +44895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1881" spans="1:6" ht="10" customHeight="1">
+    <row r="1881" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1881" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44918,7 +44915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1882" spans="1:6" ht="10" customHeight="1">
+    <row r="1882" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1882" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44938,7 +44935,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1883" spans="1:6" ht="9" customHeight="1">
+    <row r="1883" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1883" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44958,7 +44955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1884" spans="1:6" ht="10" customHeight="1">
+    <row r="1884" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1884" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44978,7 +44975,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1885" spans="1:6" ht="10" customHeight="1">
+    <row r="1885" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1885" s="2" t="s">
         <v>1630</v>
       </c>
@@ -44998,7 +44995,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1886" spans="1:6" ht="10" customHeight="1">
+    <row r="1886" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1886" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45018,7 +45015,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1887" spans="1:6" ht="10" customHeight="1">
+    <row r="1887" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1887" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45038,7 +45035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1888" spans="1:6" ht="10" customHeight="1">
+    <row r="1888" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1888" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45058,7 +45055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1889" spans="1:6" ht="10" customHeight="1">
+    <row r="1889" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1889" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45078,7 +45075,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1890" spans="1:6" ht="9" customHeight="1">
+    <row r="1890" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1890" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45098,7 +45095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1891" spans="1:6" ht="10" customHeight="1">
+    <row r="1891" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1891" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45118,7 +45115,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1892" spans="1:6" ht="9" customHeight="1">
+    <row r="1892" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1892" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45138,7 +45135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1893" spans="1:6" ht="10" customHeight="1">
+    <row r="1893" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1893" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45158,7 +45155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1894" spans="1:6" ht="10" customHeight="1">
+    <row r="1894" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1894" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45178,7 +45175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1895" spans="1:6" ht="10" customHeight="1">
+    <row r="1895" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1895" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45198,7 +45195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1896" spans="1:6" ht="10" customHeight="1">
+    <row r="1896" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1896" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45218,7 +45215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1897" spans="1:6" ht="10" customHeight="1">
+    <row r="1897" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1897" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45238,7 +45235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1898" spans="1:6" ht="9" customHeight="1">
+    <row r="1898" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1898" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45258,7 +45255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1899" spans="1:6" ht="9" customHeight="1">
+    <row r="1899" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1899" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45278,7 +45275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1900" spans="1:6" ht="10" customHeight="1">
+    <row r="1900" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1900" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45298,7 +45295,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1901" spans="1:6" ht="10" customHeight="1">
+    <row r="1901" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1901" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45318,7 +45315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1902" spans="1:6" ht="10" customHeight="1">
+    <row r="1902" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1902" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45338,7 +45335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1903" spans="1:6" ht="10" customHeight="1">
+    <row r="1903" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1903" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45358,7 +45355,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="1904" spans="1:6" ht="10" customHeight="1">
+    <row r="1904" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1904" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45378,7 +45375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1905" spans="1:6" ht="10" customHeight="1">
+    <row r="1905" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1905" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45398,7 +45395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1906" spans="1:6" ht="10" customHeight="1">
+    <row r="1906" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1906" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45418,7 +45415,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1907" spans="1:6" ht="10" customHeight="1">
+    <row r="1907" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1907" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45438,7 +45435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1908" spans="1:6" ht="10" customHeight="1">
+    <row r="1908" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1908" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45458,7 +45455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1909" spans="1:6" ht="10" customHeight="1">
+    <row r="1909" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1909" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45478,7 +45475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1910" spans="1:6" ht="10" customHeight="1">
+    <row r="1910" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1910" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45498,7 +45495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1911" spans="1:6" ht="10" customHeight="1">
+    <row r="1911" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1911" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45518,7 +45515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1912" spans="1:6" ht="10" customHeight="1">
+    <row r="1912" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1912" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45538,7 +45535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1913" spans="1:6" ht="10" customHeight="1">
+    <row r="1913" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1913" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45558,7 +45555,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1914" spans="1:6" ht="9" customHeight="1">
+    <row r="1914" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1914" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45578,7 +45575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1915" spans="1:6" ht="10" customHeight="1">
+    <row r="1915" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1915" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45598,7 +45595,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1916" spans="1:6" ht="9" customHeight="1">
+    <row r="1916" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1916" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45618,7 +45615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1917" spans="1:6" ht="10" customHeight="1">
+    <row r="1917" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1917" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45638,7 +45635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1918" spans="1:6" ht="10" customHeight="1">
+    <row r="1918" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1918" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45658,7 +45655,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1919" spans="1:6" ht="10" customHeight="1">
+    <row r="1919" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1919" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45678,7 +45675,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1920" spans="1:6" ht="9" customHeight="1">
+    <row r="1920" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1920" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45698,7 +45695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1921" spans="1:6" ht="10" customHeight="1">
+    <row r="1921" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1921" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45718,7 +45715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1922" spans="1:6" ht="10" customHeight="1">
+    <row r="1922" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1922" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45738,7 +45735,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1923" spans="1:6" ht="9" customHeight="1">
+    <row r="1923" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1923" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45758,7 +45755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1924" spans="1:6" ht="10" customHeight="1">
+    <row r="1924" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1924" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45778,7 +45775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1925" spans="1:6" ht="9" customHeight="1">
+    <row r="1925" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1925" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45798,7 +45795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1926" spans="1:6" ht="10" customHeight="1">
+    <row r="1926" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1926" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45818,7 +45815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1927" spans="1:6" ht="10" customHeight="1">
+    <row r="1927" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1927" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45838,7 +45835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1928" spans="1:6" ht="10" customHeight="1">
+    <row r="1928" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1928" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45858,7 +45855,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1929" spans="1:6" ht="10" customHeight="1">
+    <row r="1929" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1929" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45878,7 +45875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1930" spans="1:6" ht="9" customHeight="1">
+    <row r="1930" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1930" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45898,7 +45895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1931" spans="1:6" ht="10" customHeight="1">
+    <row r="1931" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1931" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45918,7 +45915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1932" spans="1:6" ht="10" customHeight="1">
+    <row r="1932" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1932" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45938,7 +45935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1933" spans="1:6" ht="9" customHeight="1">
+    <row r="1933" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1933" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45958,7 +45955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1934" spans="1:6" ht="10" customHeight="1">
+    <row r="1934" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1934" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45978,7 +45975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1935" spans="1:6" ht="10" customHeight="1">
+    <row r="1935" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1935" s="2" t="s">
         <v>1630</v>
       </c>
@@ -45998,7 +45995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1936" spans="1:6" ht="10" customHeight="1">
+    <row r="1936" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1936" s="2" t="s">
         <v>1630</v>
       </c>
@@ -46018,7 +46015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1937" spans="1:6" ht="10" customHeight="1">
+    <row r="1937" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1937" s="2" t="s">
         <v>1630</v>
       </c>
@@ -46038,7 +46035,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1938" spans="1:6" ht="10" customHeight="1">
+    <row r="1938" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1938" s="2" t="s">
         <v>1630</v>
       </c>
@@ -46058,7 +46055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1939" spans="1:6" ht="11" customHeight="1">
+    <row r="1939" spans="1:6" ht="11" hidden="1" customHeight="1">
       <c r="A1939" s="2" t="s">
         <v>1630</v>
       </c>
@@ -46078,7 +46075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1940" spans="1:6" ht="10" customHeight="1">
+    <row r="1940" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1940" s="2" t="s">
         <v>1630</v>
       </c>
@@ -46098,7 +46095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1941" spans="1:6" ht="10" customHeight="1">
+    <row r="1941" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1941" s="2" t="s">
         <v>1630</v>
       </c>
@@ -46118,7 +46115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1942" spans="1:6" ht="10" customHeight="1">
+    <row r="1942" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1942" s="2" t="s">
         <v>1630</v>
       </c>
@@ -46138,7 +46135,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="1943" spans="1:6" ht="10" customHeight="1">
+    <row r="1943" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1943" s="2" t="s">
         <v>1630</v>
       </c>
@@ -46158,7 +46155,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1944" spans="1:6" ht="10" customHeight="1">
+    <row r="1944" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1944" s="2" t="s">
         <v>1630</v>
       </c>
@@ -46178,7 +46175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1945" spans="1:6" ht="10" customHeight="1">
+    <row r="1945" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1945" s="2" t="s">
         <v>1630</v>
       </c>
@@ -46198,7 +46195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1946" spans="1:6" ht="10" customHeight="1">
+    <row r="1946" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1946" s="2" t="s">
         <v>1630</v>
       </c>
@@ -46218,7 +46215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1947" spans="1:6" ht="9" customHeight="1">
+    <row r="1947" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1947" s="2" t="s">
         <v>1630</v>
       </c>
@@ -46238,7 +46235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1948" spans="1:6" ht="10" customHeight="1">
+    <row r="1948" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1948" s="2" t="s">
         <v>1630</v>
       </c>
@@ -46258,7 +46255,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1949" spans="1:6" ht="10" customHeight="1">
+    <row r="1949" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1949" s="2" t="s">
         <v>1630</v>
       </c>
@@ -46278,7 +46275,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="1950" spans="1:6" ht="10" customHeight="1">
+    <row r="1950" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1950" s="2" t="s">
         <v>1630</v>
       </c>
@@ -46298,7 +46295,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="1951" spans="1:6" ht="9" customHeight="1">
+    <row r="1951" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1951" s="2" t="s">
         <v>1630</v>
       </c>
@@ -46318,7 +46315,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1952" spans="1:6" ht="9" customHeight="1">
+    <row r="1952" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1952" s="2" t="s">
         <v>1630</v>
       </c>
@@ -46338,7 +46335,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1953" spans="1:6" ht="9" customHeight="1">
+    <row r="1953" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1953" s="2" t="s">
         <v>1630</v>
       </c>
@@ -46358,7 +46355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1954" spans="1:6" ht="9" customHeight="1">
+    <row r="1954" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1954" s="2" t="s">
         <v>1630</v>
       </c>
@@ -46378,7 +46375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1955" spans="1:6" ht="10" customHeight="1">
+    <row r="1955" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1955" s="2" t="s">
         <v>1630</v>
       </c>
@@ -46398,7 +46395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1956" spans="1:6" ht="10" customHeight="1">
+    <row r="1956" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1956" s="2" t="s">
         <v>1630</v>
       </c>
@@ -46418,7 +46415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1957" spans="1:6" ht="10" customHeight="1">
+    <row r="1957" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1957" s="2" t="s">
         <v>1630</v>
       </c>
@@ -46438,7 +46435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1958" spans="1:6" ht="10" customHeight="1">
+    <row r="1958" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1958" s="2" t="s">
         <v>1630</v>
       </c>
@@ -46458,7 +46455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1959" spans="1:6" ht="10" customHeight="1">
+    <row r="1959" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1959" s="2" t="s">
         <v>1630</v>
       </c>
@@ -46478,7 +46475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1960" spans="1:6" ht="9" customHeight="1">
+    <row r="1960" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1960" s="2" t="s">
         <v>1630</v>
       </c>
@@ -46498,7 +46495,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="1961" spans="1:6" ht="9" customHeight="1">
+    <row r="1961" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1961" s="2" t="s">
         <v>1630</v>
       </c>
@@ -46518,7 +46515,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1962" spans="1:6" ht="9" customHeight="1">
+    <row r="1962" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1962" s="2" t="s">
         <v>1630</v>
       </c>
@@ -46538,7 +46535,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1963" spans="1:6" ht="9" customHeight="1">
+    <row r="1963" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1963" s="2" t="s">
         <v>1630</v>
       </c>
@@ -46558,7 +46555,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="1964" spans="1:6" ht="9" customHeight="1">
+    <row r="1964" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1964" s="2" t="s">
         <v>1630</v>
       </c>
@@ -46578,7 +46575,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="1965" spans="1:6" ht="9" customHeight="1">
+    <row r="1965" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1965" s="2" t="s">
         <v>1630</v>
       </c>
@@ -46598,7 +46595,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="1966" spans="1:6" ht="10" customHeight="1">
+    <row r="1966" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1966" s="2" t="s">
         <v>1630</v>
       </c>
@@ -46618,7 +46615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1967" spans="1:6" ht="11" customHeight="1">
+    <row r="1967" spans="1:6" ht="11" hidden="1" customHeight="1">
       <c r="A1967" s="2" t="s">
         <v>1630</v>
       </c>
@@ -46638,7 +46635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1968" spans="1:6" ht="9" customHeight="1">
+    <row r="1968" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1968" s="2" t="s">
         <v>1630</v>
       </c>
@@ -46658,7 +46655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1969" spans="1:6" ht="10" customHeight="1">
+    <row r="1969" spans="1:6" ht="10" hidden="1" customHeight="1">
       <c r="A1969" s="2" t="s">
         <v>1630</v>
       </c>
@@ -46678,7 +46675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1970" spans="1:6" ht="9" customHeight="1">
+    <row r="1970" spans="1:6" ht="9" hidden="1" customHeight="1">
       <c r="A1970" s="2" t="s">
         <v>1630</v>
       </c>

</xml_diff>